<commit_message>
Intermediate work on excel missing data persist
</commit_message>
<xml_diff>
--- a/downloader/custom_config/configuration.xlsx
+++ b/downloader/custom_config/configuration.xlsx
@@ -20,9 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">Nazev</t>
+  </si>
   <si>
     <t xml:space="preserve">Katalog c.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obrazek</t>
   </si>
   <si>
     <t xml:space="preserve">Popisek</t>
@@ -46,6 +52,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -66,6 +73,7 @@
       <sz val="12"/>
       <name val="Cambria"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,10 +144,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -154,21 +162,28 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="B2" s="1" t="n">
         <v>11971852</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>2</v>
+      <c r="C2" s="1"/>
+      <c r="D2" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="B3" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>3</v>
+      <c r="D3" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>